<commit_message>
added address split into three columns
</commit_message>
<xml_diff>
--- a/property_listings.xlsx
+++ b/property_listings.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb0c59427c879960/Dokumenty/UiPath/Robot4_RealEstateScraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F0DC241-3C77-4C0B-8A9E-4044166F23D8}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41480C15-72DC-4827-A2BA-DBA1AF63CE15}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{68A3964E-AA14-4F84-AC08-D41D65EA135C}"/>
   </bookViews>
   <sheets>
     <sheet name="SEATTLE" sheetId="4" r:id="rId1"/>
-    <sheet name="NEW YORK" sheetId="5" r:id="rId2"/>
+    <sheet name="NEW YORK" sheetId="9" r:id="rId2"/>
     <sheet name="Arkusz1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="305">
   <si>
     <t>Price</t>
   </si>
@@ -239,388 +239,709 @@
     <t>https://www.zillow.com/homedetails/407-Clinton-St-Bellmore-NY-11710/31391830_zpid/</t>
   </si>
   <si>
+    <t>518 30th Avenue E UNIT B, Seattle, WA 98112</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/518-30th-Ave-E-UNIT-B-Seattle-WA-98112/344517020_zpid/</t>
+  </si>
+  <si>
+    <t>1016 NE 98th Street, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1016-NE-98th-St-Seattle-WA-98115/344701795_zpid/</t>
+  </si>
+  <si>
+    <t>9515 Sand Point Way NE, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/9515-Sand-Point-Way-NE-Seattle-WA-98115/241739667_zpid/</t>
+  </si>
+  <si>
+    <t>1295 NW Elford Drive, Seattle, WA 98177</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1295-NW-Elford-Dr-Seattle-WA-98177/48790962_zpid/</t>
+  </si>
+  <si>
+    <t>8001 Jones Avenue NW, Seattle, WA 98117</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/8001-Jones-Ave-NW-Seattle-WA-98117/48976633_zpid/</t>
+  </si>
+  <si>
+    <t>2113 Aurora Avenue N, Seattle, WA 98109</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2113-Aurora-Ave-N-Seattle-WA-98109/48749445_zpid/</t>
+  </si>
+  <si>
+    <t>9014 20th Avenue NE, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/9014-20th-Ave-NE-Seattle-WA-98115/49091512_zpid/</t>
+  </si>
+  <si>
+    <t>926 NW 62nd Street, Seattle, WA 98107</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/926-NW-62nd-St-Seattle-WA-98107/344783726_zpid/</t>
+  </si>
+  <si>
+    <t>1001 NE Boat Street, Seattle, WA 98105</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1001-NE-Boat-St-Seattle-WA-98105/2057666309_zpid/</t>
+  </si>
+  <si>
+    <t>1703 37th Avenue, Seattle, WA 98122</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1703-37th-Ave-Seattle-WA-98122/49036924_zpid/</t>
+  </si>
+  <si>
+    <t>5041 47th Avenue NE UNIT 98105, Seattle, WA 98105</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/5041-47th-Ave-NE-98105-Seattle-WA-98105/344918710_zpid/</t>
+  </si>
+  <si>
+    <t>1129 N 81st Street, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1129-N-81st-St-Seattle-WA-98103/48694451_zpid/</t>
+  </si>
+  <si>
+    <t>4121 32nd Avenue SW, Seattle, WA 98126</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4121-32nd-Ave-SW-Seattle-WA-98126/108839871_zpid/</t>
+  </si>
+  <si>
+    <t>343 N 81st Street, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/343-N-81st-St-Seattle-WA-98103/48995901_zpid/</t>
+  </si>
+  <si>
+    <t>712 N 62nd Street, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/712-N-62nd-St-Seattle-WA-98103/49140266_zpid/</t>
+  </si>
+  <si>
+    <t>7558 16th Avenue SW, Seattle, WA 98106</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/7558-16th-Ave-SW-Seattle-WA-98106/48777731_zpid/</t>
+  </si>
+  <si>
+    <t>2200 N 38th Street, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2200-N-38th-St-Seattle-WA-98103/48919709_zpid/</t>
+  </si>
+  <si>
+    <t>902 NE 62nd Street, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/902-NE-62nd-St-Seattle-WA-98115/49119885_zpid/</t>
+  </si>
+  <si>
+    <t>3207 29th Avenue W, Seattle, WA 98199</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3207-29th-Ave-W-Seattle-WA-98199/49009693_zpid/</t>
+  </si>
+  <si>
+    <t>2126 33rd Avenue W, Seattle, WA 98199</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2126-33rd-Ave-W-Seattle-WA-98199/48727106_zpid/</t>
+  </si>
+  <si>
+    <t>3835 33rd Avenue SW, Seattle, WA 98126</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3835-33rd-Ave-SW-Seattle-WA-98126/49127096_zpid/</t>
+  </si>
+  <si>
+    <t>3010 NE 60th Street, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3010-NE-60th-St-Seattle-WA-98115/48765344_zpid/</t>
+  </si>
+  <si>
+    <t>7309 Winona Ave N, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/7309-Winona-Ave-N-Seattle-WA-98103/123536578_zpid/</t>
+  </si>
+  <si>
+    <t>4508 53rd Avenue NE, Seattle, WA 98105</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4508-53rd-Ave-NE-Seattle-WA-98105/344572984_zpid/</t>
+  </si>
+  <si>
+    <t>2006 28th Avenue S, Seattle, WA 98144</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2006-28th-Ave-S-Seattle-WA-98144/96669856_zpid/</t>
+  </si>
+  <si>
+    <t>3536 NE 70th Street, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3536-NE-70th-St-Seattle-WA-98115/49073769_zpid/</t>
+  </si>
+  <si>
+    <t>2538 35th Avenue W, Seattle, WA 98199</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2538-35th-Ave-W-Seattle-WA-98199/48727039_zpid/</t>
+  </si>
+  <si>
+    <t>8757 12th Avenue NW UNIT B, Seattle, WA 98117</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/8757-12th-Ave-NW-B-Seattle-WA-98117/2056042698_zpid/</t>
+  </si>
+  <si>
+    <t>4232 NE 74th Street, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4232-NE-74th-St-Seattle-WA-98115/48671738_zpid/</t>
+  </si>
+  <si>
+    <t>536 N 102nd Street, Seattle, WA 98133</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/536-N-102nd-St-Seattle-WA-98133/48984929_zpid/</t>
+  </si>
+  <si>
+    <t>1702 34th Avenue, Seattle, WA 98122</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1702-34th-Ave-Seattle-WA-98122/49046628_zpid/</t>
+  </si>
+  <si>
+    <t>4516 15th Avenue S, Seattle, WA 98108</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4516-15th-Ave-S-Seattle-WA-98108/48888041_zpid/</t>
+  </si>
+  <si>
+    <t>9257 Ashworth Avenue N UNIT B, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/9257-Ashworth-Ave-N-B-Seattle-WA-98103/344753397_zpid/</t>
+  </si>
+  <si>
+    <t>7339 18th Avenue NW, Seattle, WA 98117</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/7339-18th-Ave-NW-Seattle-WA-98117/49041306_zpid/</t>
+  </si>
+  <si>
+    <t>8755 12th Avenue NW UNIT B, Seattle, WA 98117</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/8755-12th-Ave-NW-B-Seattle-WA-98117/2056042695_zpid/</t>
+  </si>
+  <si>
+    <t>2305 24th Avenue S, Seattle, WA 98144</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2305-24th-Ave-S-Seattle-WA-98144/48744960_zpid/</t>
+  </si>
+  <si>
+    <t>1919 32nd Avenue W, Seattle, WA 98199</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1919-32nd-Ave-W-Seattle-WA-98199/48727090_zpid/</t>
+  </si>
+  <si>
+    <t>5518 Kenwood Place N, Seattle, WA 98103</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/5518-Kenwood-Pl-N-Seattle-WA-98103/49144278_zpid/</t>
+  </si>
+  <si>
+    <t>3452 14th Avenue W, Seattle, WA 98119</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3452-14th-Ave-W-Seattle-WA-98119/48825093_zpid/</t>
+  </si>
+  <si>
+    <t>4063 Letitia Avenue S, Seattle, WA 98118</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4063-Letitia-Ave-S-Seattle-WA-98118/48745433_zpid/</t>
+  </si>
+  <si>
+    <t>233 Harvard Avenue E, Seattle, WA 98102</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/233-Harvard-Ave-E-Seattle-WA-98102/48848032_zpid/</t>
+  </si>
+  <si>
+    <t>7956 Military Road S, Seattle, WA 98108</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/7956-Military-Rd-S-Seattle-WA-98108/48649330_zpid/</t>
+  </si>
+  <si>
+    <t>10710 C Whitman Avenue N, Seattle, WA 98133</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/10710C-Whitman-Ave-N-Seattle-WA-98133/48790335_zpid/</t>
+  </si>
+  <si>
+    <t>1515 McGilvra Boulevard E, Seattle, WA 98112</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1515-McGilvra-Blvd-E-Seattle-WA-98112/48956601_zpid/</t>
+  </si>
+  <si>
+    <t>10 Florentia Street, Seattle, WA 98109</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/10-Florentia-St-Seattle-WA-98109/80259848_zpid/</t>
+  </si>
+  <si>
+    <t>1628 30th Avenue, Seattle, WA 98122</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1628-30th-Ave-Seattle-WA-98122/2054360740_zpid/</t>
+  </si>
+  <si>
+    <t>1410 NW 77th Street, Seattle, WA 98117</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1410-NW-77th-St-Seattle-WA-98117/49096475_zpid/</t>
+  </si>
+  <si>
+    <t>2227 Prescott Avenue SW, Seattle, WA 98126</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/2227-Prescott-Ave-SW-Seattle-WA-98126/49124535_zpid/</t>
+  </si>
+  <si>
+    <t>4716 45th Avenue SW, Seattle, WA 98116</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4716-45th-Ave-SW-Seattle-WA-98116/48737090_zpid/</t>
+  </si>
+  <si>
+    <t>3007 S Juneau Street, Seattle, WA 98108</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3007-S-Juneau-St-Seattle-WA-98108/49063415_zpid/</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>3856 Stalker Rd, Macedon, NY 14502</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/3856-Stalker-Rd-Macedon-NY-14502/32914300_zpid/</t>
+  </si>
+  <si>
+    <t>30 Redbud Ct, East Amherst, NY 14051</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/30-Redbud-Ct-East-Amherst-NY-14051/30237744_zpid/</t>
+  </si>
+  <si>
+    <t>31 Meadow Dr, Big Flats, NY 14814</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/31-Meadow-Dr-Big-Flats-NY-14814/29962420_zpid/</t>
+  </si>
+  <si>
+    <t>36 Hathaway Rd, Rochester, NY 14617</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/36-Hathaway-Rd-Rochester-NY-14617/30970923_zpid/</t>
+  </si>
+  <si>
+    <t>1 Sunset Dr, Avon, NY 14414</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/1-Sunset-Dr-Avon-NY-14414/30806321_zpid/</t>
+  </si>
+  <si>
+    <t>66 Pickerel Road, Monroe, NY 10950</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/66-Pickerel-Rd-Monroe-NY-10950/31807123_zpid/</t>
+  </si>
+  <si>
+    <t>107 S Lincoln Ave, Liverpool, NY 13088</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/107-S-Lincoln-Ave-Liverpool-NY-13088/31769015_zpid/</t>
+  </si>
+  <si>
+    <t>4965 Driftwood Dr, Liverpool, NY 13088</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/4965-Driftwood-Dr-Liverpool-NY-13088/31770755_zpid/</t>
+  </si>
+  <si>
+    <t>214 Ardmore Street, Endicott, NY 13760</t>
+  </si>
+  <si>
+    <t>https://www.zillow.com/homedetails/214-Ardmore-St-Endicott-NY-13760/29764926_zpid/</t>
+  </si>
+  <si>
     <t>114 Fiddlers Holw, Penfield, NY 14526</t>
   </si>
   <si>
     <t>https://www.zillow.com/homedetails/114-Fiddlers-Holw-Penfield-NY-14526/70904967_zpid/</t>
   </si>
   <si>
-    <t>518 30th Avenue E UNIT B, Seattle, WA 98112</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/518-30th-Ave-E-UNIT-B-Seattle-WA-98112/344517020_zpid/</t>
-  </si>
-  <si>
-    <t>1016 NE 98th Street, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1016-NE-98th-St-Seattle-WA-98115/344701795_zpid/</t>
-  </si>
-  <si>
-    <t>9515 Sand Point Way NE, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/9515-Sand-Point-Way-NE-Seattle-WA-98115/241739667_zpid/</t>
-  </si>
-  <si>
-    <t>1295 NW Elford Drive, Seattle, WA 98177</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1295-NW-Elford-Dr-Seattle-WA-98177/48790962_zpid/</t>
-  </si>
-  <si>
-    <t>8001 Jones Avenue NW, Seattle, WA 98117</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/8001-Jones-Ave-NW-Seattle-WA-98117/48976633_zpid/</t>
-  </si>
-  <si>
-    <t>2113 Aurora Avenue N, Seattle, WA 98109</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2113-Aurora-Ave-N-Seattle-WA-98109/48749445_zpid/</t>
-  </si>
-  <si>
-    <t>9014 20th Avenue NE, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/9014-20th-Ave-NE-Seattle-WA-98115/49091512_zpid/</t>
-  </si>
-  <si>
-    <t>926 NW 62nd Street, Seattle, WA 98107</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/926-NW-62nd-St-Seattle-WA-98107/344783726_zpid/</t>
-  </si>
-  <si>
-    <t>1001 NE Boat Street, Seattle, WA 98105</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1001-NE-Boat-St-Seattle-WA-98105/2057666309_zpid/</t>
-  </si>
-  <si>
-    <t>1703 37th Avenue, Seattle, WA 98122</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1703-37th-Ave-Seattle-WA-98122/49036924_zpid/</t>
-  </si>
-  <si>
-    <t>5041 47th Avenue NE UNIT 98105, Seattle, WA 98105</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/5041-47th-Ave-NE-98105-Seattle-WA-98105/344918710_zpid/</t>
-  </si>
-  <si>
-    <t>1129 N 81st Street, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1129-N-81st-St-Seattle-WA-98103/48694451_zpid/</t>
-  </si>
-  <si>
-    <t>4121 32nd Avenue SW, Seattle, WA 98126</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4121-32nd-Ave-SW-Seattle-WA-98126/108839871_zpid/</t>
-  </si>
-  <si>
-    <t>343 N 81st Street, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/343-N-81st-St-Seattle-WA-98103/48995901_zpid/</t>
-  </si>
-  <si>
-    <t>712 N 62nd Street, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/712-N-62nd-St-Seattle-WA-98103/49140266_zpid/</t>
-  </si>
-  <si>
-    <t>7558 16th Avenue SW, Seattle, WA 98106</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/7558-16th-Ave-SW-Seattle-WA-98106/48777731_zpid/</t>
-  </si>
-  <si>
-    <t>2200 N 38th Street, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2200-N-38th-St-Seattle-WA-98103/48919709_zpid/</t>
-  </si>
-  <si>
-    <t>902 NE 62nd Street, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/902-NE-62nd-St-Seattle-WA-98115/49119885_zpid/</t>
-  </si>
-  <si>
-    <t>3207 29th Avenue W, Seattle, WA 98199</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/3207-29th-Ave-W-Seattle-WA-98199/49009693_zpid/</t>
-  </si>
-  <si>
-    <t>2126 33rd Avenue W, Seattle, WA 98199</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2126-33rd-Ave-W-Seattle-WA-98199/48727106_zpid/</t>
-  </si>
-  <si>
-    <t>3835 33rd Avenue SW, Seattle, WA 98126</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/3835-33rd-Ave-SW-Seattle-WA-98126/49127096_zpid/</t>
-  </si>
-  <si>
-    <t>3010 NE 60th Street, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/3010-NE-60th-St-Seattle-WA-98115/48765344_zpid/</t>
-  </si>
-  <si>
-    <t>7309 Winona Ave N, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/7309-Winona-Ave-N-Seattle-WA-98103/123536578_zpid/</t>
-  </si>
-  <si>
-    <t>4508 53rd Avenue NE, Seattle, WA 98105</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4508-53rd-Ave-NE-Seattle-WA-98105/344572984_zpid/</t>
-  </si>
-  <si>
-    <t>2006 28th Avenue S, Seattle, WA 98144</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2006-28th-Ave-S-Seattle-WA-98144/96669856_zpid/</t>
-  </si>
-  <si>
-    <t>3536 NE 70th Street, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/3536-NE-70th-St-Seattle-WA-98115/49073769_zpid/</t>
-  </si>
-  <si>
-    <t>2538 35th Avenue W, Seattle, WA 98199</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2538-35th-Ave-W-Seattle-WA-98199/48727039_zpid/</t>
-  </si>
-  <si>
-    <t>8757 12th Avenue NW UNIT B, Seattle, WA 98117</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/8757-12th-Ave-NW-B-Seattle-WA-98117/2056042698_zpid/</t>
-  </si>
-  <si>
-    <t>4232 NE 74th Street, Seattle, WA 98115</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4232-NE-74th-St-Seattle-WA-98115/48671738_zpid/</t>
-  </si>
-  <si>
-    <t>536 N 102nd Street, Seattle, WA 98133</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/536-N-102nd-St-Seattle-WA-98133/48984929_zpid/</t>
-  </si>
-  <si>
-    <t>1702 34th Avenue, Seattle, WA 98122</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1702-34th-Ave-Seattle-WA-98122/49046628_zpid/</t>
-  </si>
-  <si>
-    <t>4516 15th Avenue S, Seattle, WA 98108</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4516-15th-Ave-S-Seattle-WA-98108/48888041_zpid/</t>
-  </si>
-  <si>
-    <t>9257 Ashworth Avenue N UNIT B, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/9257-Ashworth-Ave-N-B-Seattle-WA-98103/344753397_zpid/</t>
-  </si>
-  <si>
-    <t>7339 18th Avenue NW, Seattle, WA 98117</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/7339-18th-Ave-NW-Seattle-WA-98117/49041306_zpid/</t>
-  </si>
-  <si>
-    <t>8755 12th Avenue NW UNIT B, Seattle, WA 98117</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/8755-12th-Ave-NW-B-Seattle-WA-98117/2056042695_zpid/</t>
-  </si>
-  <si>
-    <t>2305 24th Avenue S, Seattle, WA 98144</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2305-24th-Ave-S-Seattle-WA-98144/48744960_zpid/</t>
-  </si>
-  <si>
-    <t>1919 32nd Avenue W, Seattle, WA 98199</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1919-32nd-Ave-W-Seattle-WA-98199/48727090_zpid/</t>
-  </si>
-  <si>
-    <t>5518 Kenwood Place N, Seattle, WA 98103</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/5518-Kenwood-Pl-N-Seattle-WA-98103/49144278_zpid/</t>
-  </si>
-  <si>
-    <t>3452 14th Avenue W, Seattle, WA 98119</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/3452-14th-Ave-W-Seattle-WA-98119/48825093_zpid/</t>
-  </si>
-  <si>
-    <t>4063 Letitia Avenue S, Seattle, WA 98118</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4063-Letitia-Ave-S-Seattle-WA-98118/48745433_zpid/</t>
-  </si>
-  <si>
-    <t>233 Harvard Avenue E, Seattle, WA 98102</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/233-Harvard-Ave-E-Seattle-WA-98102/48848032_zpid/</t>
-  </si>
-  <si>
-    <t>7956 Military Road S, Seattle, WA 98108</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/7956-Military-Rd-S-Seattle-WA-98108/48649330_zpid/</t>
-  </si>
-  <si>
-    <t>10710 C Whitman Avenue N, Seattle, WA 98133</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/10710C-Whitman-Ave-N-Seattle-WA-98133/48790335_zpid/</t>
-  </si>
-  <si>
-    <t>1515 McGilvra Boulevard E, Seattle, WA 98112</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1515-McGilvra-Blvd-E-Seattle-WA-98112/48956601_zpid/</t>
-  </si>
-  <si>
-    <t>10 Florentia Street, Seattle, WA 98109</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/10-Florentia-St-Seattle-WA-98109/80259848_zpid/</t>
-  </si>
-  <si>
-    <t>1628 30th Avenue, Seattle, WA 98122</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1628-30th-Ave-Seattle-WA-98122/2054360740_zpid/</t>
-  </si>
-  <si>
-    <t>1410 NW 77th Street, Seattle, WA 98117</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1410-NW-77th-St-Seattle-WA-98117/49096475_zpid/</t>
-  </si>
-  <si>
-    <t>2227 Prescott Avenue SW, Seattle, WA 98126</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/2227-Prescott-Ave-SW-Seattle-WA-98126/49124535_zpid/</t>
-  </si>
-  <si>
-    <t>4716 45th Avenue SW, Seattle, WA 98116</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4716-45th-Ave-SW-Seattle-WA-98116/48737090_zpid/</t>
-  </si>
-  <si>
-    <t>3007 S Juneau Street, Seattle, WA 98108</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/3007-S-Juneau-St-Seattle-WA-98108/49063415_zpid/</t>
-  </si>
-  <si>
-    <t>618 Viewland Drive, Yorktown Heights, NY 10598</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/618-Viewland-Dr-Yorktown-Heights-NY-10598/58428553_zpid/</t>
-  </si>
-  <si>
-    <t>1912 Stuyvesant Avenue, East Meadow, NY 11554</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1912-Stuyvesant-Ave-East-Meadow-NY-11554/31325826_zpid/</t>
-  </si>
-  <si>
-    <t>5360 Golly Rd, Rome, NY 13440</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/5360-Golly-Rd-Rome-NY-13440/143314390_zpid/</t>
-  </si>
-  <si>
-    <t>35 Daniel Ave, Cheektowaga, NY 14225</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/35-Daniel-Ave-Cheektowaga-NY-14225/30294374_zpid/</t>
-  </si>
-  <si>
-    <t>433 Richard Ave, Staten Island, NY 10309</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/433-Richard-Ave-Staten-Island-NY-10309/32374557_zpid/</t>
-  </si>
-  <si>
-    <t>50 Latham Ridge Road, Latham, NY 12110</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/50-Latham-Ridge-Rd-Latham-NY-12110/29687633_zpid/</t>
-  </si>
-  <si>
-    <t>5171 Military Rd, Lewiston, NY 14092</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/5171-Military-Rd-Lewiston-NY-14092/60196971_zpid/</t>
-  </si>
-  <si>
-    <t>39 Selkirk Dr, Rochester, NY 14626</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/39-Selkirk-Dr-Rochester-NY-14626/30946615_zpid/</t>
-  </si>
-  <si>
-    <t>26 Torrington Dr, Rochester, NY 14618</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/26-Torrington-Dr-Rochester-NY-14618/237423419_zpid/</t>
-  </si>
-  <si>
-    <t>9 Salem Road, Pound Ridge, NY 10576</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/9-Salem-Rd-Pound-Ridge-NY-10576/33084092_zpid/</t>
-  </si>
-  <si>
-    <t>7682 County Road 42, Victor, NY 14564</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/7682-County-Road-42-Victor-NY-14564/31900774_zpid/</t>
-  </si>
-  <si>
-    <t>393 N Rockingham Way, Amherst, NY 14228</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/393-N-Rockingham-Way-Amherst-NY-14228/98058622_zpid/</t>
-  </si>
-  <si>
-    <t>311 Gordon Ave, Mattydale, NY 13211</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/311-Gordon-Ave-Mattydale-NY-13211/31774104_zpid/</t>
+    <t>65 Green Street</t>
+  </si>
+  <si>
+    <t>11 Clearwater Road</t>
+  </si>
+  <si>
+    <t>4 Wilderness Road</t>
+  </si>
+  <si>
+    <t>133 Clearvale Dr</t>
+  </si>
+  <si>
+    <t>89 Harvest Rd</t>
+  </si>
+  <si>
+    <t>48 Chapin St</t>
+  </si>
+  <si>
+    <t>3856 Stalker Rd</t>
+  </si>
+  <si>
+    <t>30 Redbud Ct</t>
+  </si>
+  <si>
+    <t>31 Meadow Dr</t>
+  </si>
+  <si>
+    <t>36 Hathaway Rd</t>
+  </si>
+  <si>
+    <t>1 Sunset Dr</t>
+  </si>
+  <si>
+    <t>66 Pickerel Road</t>
+  </si>
+  <si>
+    <t>107 S Lincoln Ave</t>
+  </si>
+  <si>
+    <t>4965 Driftwood Dr</t>
+  </si>
+  <si>
+    <t>5626 Newhouse Rd</t>
+  </si>
+  <si>
+    <t>214 Ardmore Street</t>
+  </si>
+  <si>
+    <t>329 E 9th St</t>
+  </si>
+  <si>
+    <t>7 Margaret Drive</t>
+  </si>
+  <si>
+    <t>206 Sweetman Road</t>
+  </si>
+  <si>
+    <t>219 Aris Ave</t>
+  </si>
+  <si>
+    <t>67 Brewster St</t>
+  </si>
+  <si>
+    <t>201 Dale St</t>
+  </si>
+  <si>
+    <t>305 Valley Green Dr</t>
+  </si>
+  <si>
+    <t>1097 Marcia Dr</t>
+  </si>
+  <si>
+    <t>6 Sheila Drive</t>
+  </si>
+  <si>
+    <t>19 White Fawn Run</t>
+  </si>
+  <si>
+    <t>141 Brannon Ln</t>
+  </si>
+  <si>
+    <t>8210 Perrugia Ln</t>
+  </si>
+  <si>
+    <t>7364 E Seneca Tpke</t>
+  </si>
+  <si>
+    <t>166 Cayuga St</t>
+  </si>
+  <si>
+    <t>54 Taylor Dr</t>
+  </si>
+  <si>
+    <t>1366 County Road 30</t>
+  </si>
+  <si>
+    <t>21 Marc Mar Cir</t>
+  </si>
+  <si>
+    <t>1302 Sausse Avenue</t>
+  </si>
+  <si>
+    <t>6778 Lake Ave</t>
+  </si>
+  <si>
+    <t>4057 Ridge Chapel Rd</t>
+  </si>
+  <si>
+    <t>308 Poillon Ave</t>
+  </si>
+  <si>
+    <t>74 Birchwood Lane</t>
+  </si>
+  <si>
+    <t>1289 Plank Road</t>
+  </si>
+  <si>
+    <t>4575 Ridge Chapel Rd</t>
+  </si>
+  <si>
+    <t>407 Clinton St</t>
+  </si>
+  <si>
+    <t>114 Fiddlers Holw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hudson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 12534</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Highland</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 12528</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nissequogue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 11780</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cheektowaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14225</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fairport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14450</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Canandaigua</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14424</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Macedon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> East Amherst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14051</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Big Flats</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14814</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rochester</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14617</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Avon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14414</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monroe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 10950</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liverpool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13088</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Endicott</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13760</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oswego</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13126</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ballston Spa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 12020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14206</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Staten Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 10304</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Syracuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13208</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Penfield</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14526</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> North Tonawanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14120</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Syosset</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 11791</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14624</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Webster</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14580</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13041</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manlius</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13104</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 13073</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tonawanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14150</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Andover</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14806</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14606</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Troy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 12180</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Williamson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14589</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 14505</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 10312</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Schenectady</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 12309</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Forestburgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 12777</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bellmore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NY 11710</t>
   </si>
 </sst>
 </file>
@@ -657,8 +978,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -685,6 +1007,26 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1025,10 +1367,10 @@
         <v>702</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1045,10 +1387,10 @@
         <v>1081</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1065,10 +1407,10 @@
         <v>3674</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1085,10 +1427,10 @@
         <v>7362</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,10 +1447,10 @@
         <v>2060</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1125,10 +1467,10 @@
         <v>2460</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1145,10 +1487,10 @@
         <v>1150</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1165,10 +1507,10 @@
         <v>1097</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,10 +1527,10 @@
         <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,10 +1547,10 @@
         <v>1820</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,10 +1567,10 @@
         <v>1710</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1245,10 +1587,10 @@
         <v>1196</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1265,10 +1607,10 @@
         <v>1600</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,10 +1627,10 @@
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1305,10 +1647,10 @@
         <v>2000</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1325,10 +1667,10 @@
         <v>990</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1345,10 +1687,10 @@
         <v>2845</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1365,10 +1707,10 @@
         <v>1840</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1385,10 +1727,10 @@
         <v>3080</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1405,10 +1747,10 @@
         <v>2700</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1425,10 +1767,10 @@
         <v>2210</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,10 +1787,10 @@
         <v>2640</v>
       </c>
       <c r="E23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,10 +1807,10 @@
         <v>640</v>
       </c>
       <c r="E24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,10 +1827,10 @@
         <v>3703</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,10 +1847,10 @@
         <v>2830</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,10 +1867,10 @@
         <v>1550</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,10 +1887,10 @@
         <v>4400</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,10 +1907,10 @@
         <v>852</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1585,10 +1927,10 @@
         <v>2660</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,10 +1947,10 @@
         <v>550</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,10 +1967,10 @@
         <v>2800</v>
       </c>
       <c r="E32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,10 +1987,10 @@
         <v>1400</v>
       </c>
       <c r="E33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1665,10 +2007,10 @@
         <v>650</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1685,10 +2027,10 @@
         <v>2018</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,10 +2047,10 @@
         <v>812</v>
       </c>
       <c r="E36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,10 +2067,10 @@
         <v>1200</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1745,10 +2087,10 @@
         <v>420</v>
       </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1765,10 +2107,10 @@
         <v>1690</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1785,10 +2127,10 @@
         <v>1530</v>
       </c>
       <c r="E40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1805,10 +2147,10 @@
         <v>1290</v>
       </c>
       <c r="E41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1825,10 +2167,10 @@
         <v>3556</v>
       </c>
       <c r="E42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,10 +2187,10 @@
         <v>2900</v>
       </c>
       <c r="E43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,10 +2207,10 @@
         <v>1890</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,10 +2227,10 @@
         <v>3584</v>
       </c>
       <c r="E45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1905,10 +2247,10 @@
         <v>1850</v>
       </c>
       <c r="E46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F46" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,10 +2267,10 @@
         <v>4227</v>
       </c>
       <c r="E47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F47" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,10 +2287,10 @@
         <v>1405</v>
       </c>
       <c r="E48" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F48" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,10 +2307,10 @@
         <v>3390</v>
       </c>
       <c r="E49" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F49" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1985,10 +2327,10 @@
         <v>1974</v>
       </c>
       <c r="E50" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F50" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2005,10 +2347,10 @@
         <v>2660</v>
       </c>
       <c r="E51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2017,14 +2359,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F1E41F-4D3A-4A8D-8C88-1D264DA935D2}">
-  <dimension ref="A1:F47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E71F728-223C-45CF-BF0A-FC95AC54B3C5}">
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="8" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2040,11 +2385,20 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>515000</v>
       </c>
@@ -2060,11 +2414,20 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>850000</v>
       </c>
@@ -2080,11 +2443,20 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1399000</v>
       </c>
@@ -2100,11 +2472,20 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>149900</v>
       </c>
@@ -2120,11 +2501,20 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>199000</v>
       </c>
@@ -2140,11 +2530,20 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>189900</v>
       </c>
@@ -2160,808 +2559,1148 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>80000</v>
+        <v>179900</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1240</v>
+        <v>1408</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>229900</v>
+        <v>249900</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>936</v>
+        <v>2520</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>289900</v>
+        <v>219900</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>1332</v>
+        <v>2390</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>179900</v>
+        <v>199000</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
+        <v>1355</v>
+      </c>
+      <c r="E11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>199900</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1350</v>
+      </c>
+      <c r="E12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>515000</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1700</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>300000</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2148</v>
+      </c>
+      <c r="E14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>186000</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1080</v>
+      </c>
+      <c r="E15" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>186000</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1080</v>
+      </c>
+      <c r="E16" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>189900</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>936</v>
+      </c>
+      <c r="E17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>199900</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>960</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>169000</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>80000</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>1240</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>229900</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>936</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>289900</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>1332</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>179900</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>990</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E23" t="s">
         <v>24</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F23" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>748000</v>
       </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
         <v>2227</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E24" t="s">
         <v>26</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F24" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="I24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>159900</v>
       </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D25">
         <v>1188</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E25" t="s">
         <v>28</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F25" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>279000</v>
       </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
         <v>1824</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E26" t="s">
         <v>30</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F26" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>199900</v>
       </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
         <v>1222</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E27" t="s">
         <v>32</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>1100000</v>
       </c>
-      <c r="B16">
+      <c r="B28">
         <v>5</v>
       </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
         <v>2659</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F28" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>250000</v>
       </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
         <v>1789</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E29" t="s">
         <v>36</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>289900</v>
       </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
         <v>1347</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E30" t="s">
         <v>38</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>285000</v>
       </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
         <v>1400</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E31" t="s">
         <v>40</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F31" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>199900</v>
       </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D32">
         <v>960</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E32" t="s">
         <v>42</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F32" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>369900</v>
       </c>
-      <c r="B21">
+      <c r="B33">
         <v>5</v>
       </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
         <v>2450</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E33" t="s">
         <v>44</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F33" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>248000</v>
       </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
         <v>1666</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E34" t="s">
         <v>46</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>249900</v>
       </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
         <v>1324</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E35" t="s">
         <v>48</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>164900</v>
       </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
         <v>1656</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E36" t="s">
         <v>50</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F36" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I36" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>389900</v>
       </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
         <v>2738</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E37" t="s">
         <v>52</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F37" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>264900</v>
       </c>
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
         <v>1700</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E38" t="s">
         <v>54</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F38" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="I38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>149900</v>
       </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="D39">
         <v>1547</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E39" t="s">
         <v>56</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F39" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>99900</v>
       </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
         <v>1966</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E40" t="s">
         <v>58</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F40" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>1388000</v>
       </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
         <v>2700</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E41" t="s">
         <v>60</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>225000</v>
       </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
         <v>1408</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E42" t="s">
         <v>62</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F42" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>699000</v>
       </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
         <v>2040</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E43" t="s">
         <v>64</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F43" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>209900</v>
       </c>
-      <c r="B32">
+      <c r="B44">
         <v>5</v>
       </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
         <v>1800</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E44" t="s">
         <v>66</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F44" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>255000</v>
       </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
         <v>1428</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E45" t="s">
         <v>68</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F45" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I45" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>579900</v>
       </c>
-      <c r="B34">
+      <c r="B46">
         <v>5</v>
       </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34">
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
         <v>3191</v>
       </c>
-      <c r="E34" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>799900</v>
-      </c>
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-      <c r="D35">
-        <v>2938</v>
-      </c>
-      <c r="E35" t="s">
-        <v>172</v>
-      </c>
-      <c r="F35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>788000</v>
-      </c>
-      <c r="B36">
-        <v>4</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>2851</v>
-      </c>
-      <c r="E36" t="s">
-        <v>174</v>
-      </c>
-      <c r="F36" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>62000</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>2200</v>
-      </c>
-      <c r="E37" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>224900</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <v>1130</v>
-      </c>
-      <c r="E38" t="s">
-        <v>178</v>
-      </c>
-      <c r="F38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>700000</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39">
-        <v>1800</v>
-      </c>
-      <c r="E39" t="s">
-        <v>180</v>
-      </c>
-      <c r="F39" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>299900</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>1161</v>
-      </c>
-      <c r="E40" t="s">
-        <v>182</v>
-      </c>
-      <c r="F40" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>425000</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-      <c r="D41">
-        <v>2419</v>
-      </c>
-      <c r="E41" t="s">
-        <v>184</v>
-      </c>
-      <c r="F41" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>200000</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>1873</v>
-      </c>
-      <c r="E42" t="s">
-        <v>186</v>
-      </c>
-      <c r="F42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>259900</v>
-      </c>
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>1580</v>
-      </c>
-      <c r="E43" t="s">
-        <v>188</v>
-      </c>
-      <c r="F43" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>965000</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44">
-        <v>3</v>
-      </c>
-      <c r="D44">
-        <v>2284</v>
-      </c>
-      <c r="E44" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E46" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>340000</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>2194</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="F46" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="I46" t="s">
         <v>192</v>
-      </c>
-      <c r="F45" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>799900</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>5</v>
-      </c>
-      <c r="D46">
-        <v>3285</v>
-      </c>
-      <c r="E46" t="s">
-        <v>194</v>
-      </c>
-      <c r="F46" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>149900</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>960</v>
-      </c>
-      <c r="E47" t="s">
-        <v>196</v>
-      </c>
-      <c r="F47" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed zip column type
</commit_message>
<xml_diff>
--- a/property_listings.xlsx
+++ b/property_listings.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb0c59427c879960/Dokumenty/UiPath/Robot4_RealEstateScraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{630DAE74-4378-4B6A-AB24-8D2F6F8B4A61}"/>
+  <xr:revisionPtr revIDLastSave="575" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A32695-B519-4340-B03F-AD440D60B49A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{68A3964E-AA14-4F84-AC08-D41D65EA135C}"/>
   </bookViews>
   <sheets>
     <sheet name="SEATTLE" sheetId="4" r:id="rId1"/>
-    <sheet name="NEW YORK" sheetId="10" r:id="rId2"/>
+    <sheet name="NEW YORK" sheetId="12" r:id="rId2"/>
     <sheet name="Arkusz1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="268">
   <si>
     <t>Price</t>
   </si>
@@ -644,71 +644,211 @@
     <t>Hudson</t>
   </si>
   <si>
-    <t>NY 12534</t>
-  </si>
-  <si>
     <t>Highland</t>
   </si>
   <si>
-    <t>NY 12528</t>
-  </si>
-  <si>
     <t>Nissequogue</t>
   </si>
   <si>
-    <t>NY 11780</t>
-  </si>
-  <si>
     <t>Cheektowaga</t>
   </si>
   <si>
-    <t>NY 14225</t>
-  </si>
-  <si>
     <t>Fairport</t>
   </si>
   <si>
-    <t>NY 14450</t>
-  </si>
-  <si>
     <t>Canandaigua</t>
   </si>
   <si>
-    <t>NY 14424</t>
-  </si>
-  <si>
     <t>Macedon</t>
   </si>
   <si>
-    <t>NY 14502</t>
-  </si>
-  <si>
     <t>East Amherst</t>
   </si>
   <si>
-    <t>NY 14051</t>
-  </si>
-  <si>
     <t>Big Flats</t>
   </si>
   <si>
-    <t>NY 14814</t>
-  </si>
-  <si>
     <t>Rochester</t>
   </si>
   <si>
-    <t>NY 14617</t>
+    <t>Avon</t>
+  </si>
+  <si>
+    <t>66 Pickerel Road</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>107 S Lincoln Ave</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>4965 Driftwood Dr</t>
+  </si>
+  <si>
+    <t>5626 Newhouse Rd</t>
+  </si>
+  <si>
+    <t>214 Ardmore Street</t>
+  </si>
+  <si>
+    <t>Endicott</t>
+  </si>
+  <si>
+    <t>329 E 9th St</t>
+  </si>
+  <si>
+    <t>Oswego</t>
+  </si>
+  <si>
+    <t>7 Margaret Drive</t>
+  </si>
+  <si>
+    <t>Ballston Spa</t>
+  </si>
+  <si>
+    <t>206 Sweetman Road</t>
+  </si>
+  <si>
+    <t>219 Aris Ave</t>
+  </si>
+  <si>
+    <t>67 Brewster St</t>
+  </si>
+  <si>
+    <t>Staten Island</t>
+  </si>
+  <si>
+    <t>201 Dale St</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>305 Valley Green Dr</t>
+  </si>
+  <si>
+    <t>Penfield</t>
+  </si>
+  <si>
+    <t>1097 Marcia Dr</t>
+  </si>
+  <si>
+    <t>North Tonawanda</t>
+  </si>
+  <si>
+    <t>6 Sheila Drive</t>
+  </si>
+  <si>
+    <t>Syosset</t>
+  </si>
+  <si>
+    <t>19 White Fawn Run</t>
+  </si>
+  <si>
+    <t>141 Brannon Ln</t>
+  </si>
+  <si>
+    <t>Webster</t>
+  </si>
+  <si>
+    <t>8210 Perrugia Ln</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>7364 E Seneca Tpke</t>
+  </si>
+  <si>
+    <t>Manlius</t>
+  </si>
+  <si>
+    <t>166 Cayuga St</t>
+  </si>
+  <si>
+    <t>Groton</t>
+  </si>
+  <si>
+    <t>54 Taylor Dr</t>
+  </si>
+  <si>
+    <t>Tonawanda</t>
+  </si>
+  <si>
+    <t>1366 County Road 30</t>
+  </si>
+  <si>
+    <t>Andover</t>
+  </si>
+  <si>
+    <t>21 Marc Mar Cir</t>
+  </si>
+  <si>
+    <t>1302 Sausse Avenue</t>
+  </si>
+  <si>
+    <t>Troy</t>
+  </si>
+  <si>
+    <t>6778 Lake Ave</t>
+  </si>
+  <si>
+    <t>Williamson</t>
+  </si>
+  <si>
+    <t>4057 Ridge Chapel Rd</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>308 Poillon Ave</t>
+  </si>
+  <si>
+    <t>74 Birchwood Lane</t>
+  </si>
+  <si>
+    <t>Schenectady</t>
+  </si>
+  <si>
+    <t>1289 Plank Road</t>
+  </si>
+  <si>
+    <t>Forestburgh</t>
+  </si>
+  <si>
+    <t>4575 Ridge Chapel Rd</t>
+  </si>
+  <si>
+    <t>407 Clinton St</t>
+  </si>
+  <si>
+    <t>Bellmore</t>
+  </si>
+  <si>
+    <t>114 Fiddlers Holw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -735,9 +875,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -788,6 +929,14 @@
 </file>
 
 <file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person9.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2120,14 +2269,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0ACF09-94CE-4A54-BA5A-F15E3DA2B88D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED6A5AB-D69D-4B16-979E-F1DDC0300BBB}">
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="8" width="9.140625" style="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2152,7 +2302,7 @@
       <c r="G1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>172</v>
       </c>
       <c r="I1" t="s">
@@ -2181,8 +2331,8 @@
       <c r="G2" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>205</v>
+      <c r="H2" s="2">
+        <v>12534</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -2208,10 +2358,10 @@
         <v>194</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="H3" s="2">
+        <v>12528</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>
@@ -2237,10 +2387,10 @@
         <v>195</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
+      </c>
+      <c r="H4" s="2">
+        <v>11780</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -2266,10 +2416,10 @@
         <v>196</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="H5" s="2">
+        <v>14225</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
@@ -2295,10 +2445,10 @@
         <v>197</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="H6" s="2">
+        <v>14450</v>
       </c>
       <c r="I6" t="s">
         <v>15</v>
@@ -2324,10 +2474,10 @@
         <v>198</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
+      </c>
+      <c r="H7" s="2">
+        <v>14424</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -2353,10 +2503,10 @@
         <v>199</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
+      </c>
+      <c r="H8" s="2">
+        <v>14502</v>
       </c>
       <c r="I8" t="s">
         <v>174</v>
@@ -2382,10 +2532,10 @@
         <v>200</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
+      </c>
+      <c r="H9" s="2">
+        <v>14051</v>
       </c>
       <c r="I9" t="s">
         <v>176</v>
@@ -2411,10 +2561,10 @@
         <v>201</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
+      </c>
+      <c r="H10" s="2">
+        <v>14814</v>
       </c>
       <c r="I10" t="s">
         <v>178</v>
@@ -2440,10 +2590,10 @@
         <v>202</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
+      </c>
+      <c r="H11" s="2">
+        <v>14617</v>
       </c>
       <c r="I11" t="s">
         <v>180</v>
@@ -2468,6 +2618,12 @@
       <c r="F12" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H12" s="2">
+        <v>14414</v>
+      </c>
       <c r="I12" t="s">
         <v>182</v>
       </c>
@@ -2488,6 +2644,15 @@
       <c r="E13" t="s">
         <v>6</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="2">
+        <v>12534</v>
+      </c>
       <c r="I13" t="s">
         <v>7</v>
       </c>
@@ -2508,6 +2673,15 @@
       <c r="E14" t="s">
         <v>183</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="2">
+        <v>10950</v>
+      </c>
       <c r="I14" t="s">
         <v>184</v>
       </c>
@@ -2528,6 +2702,15 @@
       <c r="E15" t="s">
         <v>185</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15" s="2">
+        <v>13088</v>
+      </c>
       <c r="I15" t="s">
         <v>186</v>
       </c>
@@ -2548,6 +2731,15 @@
       <c r="E16" t="s">
         <v>185</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H16" s="2">
+        <v>13088</v>
+      </c>
       <c r="I16" t="s">
         <v>186</v>
       </c>
@@ -2568,6 +2760,15 @@
       <c r="E17" t="s">
         <v>187</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H17" s="2">
+        <v>13088</v>
+      </c>
       <c r="I17" t="s">
         <v>188</v>
       </c>
@@ -2588,6 +2789,15 @@
       <c r="E18" t="s">
         <v>42</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H18" s="2">
+        <v>14051</v>
+      </c>
       <c r="I18" t="s">
         <v>43</v>
       </c>
@@ -2608,6 +2818,15 @@
       <c r="E19" t="s">
         <v>189</v>
       </c>
+      <c r="F19" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H19" s="2">
+        <v>13760</v>
+      </c>
       <c r="I19" t="s">
         <v>190</v>
       </c>
@@ -2628,6 +2847,15 @@
       <c r="E20" t="s">
         <v>18</v>
       </c>
+      <c r="F20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H20" s="2">
+        <v>13126</v>
+      </c>
       <c r="I20" t="s">
         <v>19</v>
       </c>
@@ -2648,6 +2876,15 @@
       <c r="E21" t="s">
         <v>20</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H21" s="2">
+        <v>12020</v>
+      </c>
       <c r="I21" t="s">
         <v>21</v>
       </c>
@@ -2668,6 +2905,15 @@
       <c r="E22" t="s">
         <v>22</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H22" s="2">
+        <v>12020</v>
+      </c>
       <c r="I22" t="s">
         <v>23</v>
       </c>
@@ -2688,6 +2934,15 @@
       <c r="E23" t="s">
         <v>24</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H23" s="2">
+        <v>14206</v>
+      </c>
       <c r="I23" t="s">
         <v>25</v>
       </c>
@@ -2708,6 +2963,15 @@
       <c r="E24" t="s">
         <v>26</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H24" s="2">
+        <v>10304</v>
+      </c>
       <c r="I24" t="s">
         <v>27</v>
       </c>
@@ -2728,6 +2992,15 @@
       <c r="E25" t="s">
         <v>28</v>
       </c>
+      <c r="F25" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H25" s="2">
+        <v>13208</v>
+      </c>
       <c r="I25" t="s">
         <v>29</v>
       </c>
@@ -2748,6 +3021,15 @@
       <c r="E26" t="s">
         <v>30</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H26" s="2">
+        <v>14526</v>
+      </c>
       <c r="I26" t="s">
         <v>31</v>
       </c>
@@ -2768,6 +3050,15 @@
       <c r="E27" t="s">
         <v>32</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H27" s="2">
+        <v>14120</v>
+      </c>
       <c r="I27" t="s">
         <v>33</v>
       </c>
@@ -2788,6 +3079,15 @@
       <c r="E28" t="s">
         <v>34</v>
       </c>
+      <c r="F28" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H28" s="2">
+        <v>11791</v>
+      </c>
       <c r="I28" t="s">
         <v>35</v>
       </c>
@@ -2808,6 +3108,15 @@
       <c r="E29" t="s">
         <v>36</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H29" s="2">
+        <v>14624</v>
+      </c>
       <c r="I29" t="s">
         <v>37</v>
       </c>
@@ -2828,6 +3137,15 @@
       <c r="E30" t="s">
         <v>38</v>
       </c>
+      <c r="F30" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H30" s="2">
+        <v>14580</v>
+      </c>
       <c r="I30" t="s">
         <v>39</v>
       </c>
@@ -2848,6 +3166,15 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
+      <c r="F31" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H31" s="2">
+        <v>13041</v>
+      </c>
       <c r="I31" t="s">
         <v>41</v>
       </c>
@@ -2868,6 +3195,15 @@
       <c r="E32" t="s">
         <v>42</v>
       </c>
+      <c r="F32" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H32" s="2">
+        <v>14051</v>
+      </c>
       <c r="I32" t="s">
         <v>43</v>
       </c>
@@ -2888,6 +3224,15 @@
       <c r="E33" t="s">
         <v>44</v>
       </c>
+      <c r="F33" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H33" s="2">
+        <v>13104</v>
+      </c>
       <c r="I33" t="s">
         <v>45</v>
       </c>
@@ -2908,6 +3253,15 @@
       <c r="E34" t="s">
         <v>46</v>
       </c>
+      <c r="F34" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H34" s="2">
+        <v>13073</v>
+      </c>
       <c r="I34" t="s">
         <v>47</v>
       </c>
@@ -2928,6 +3282,15 @@
       <c r="E35" t="s">
         <v>48</v>
       </c>
+      <c r="F35" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H35" s="2">
+        <v>14150</v>
+      </c>
       <c r="I35" t="s">
         <v>49</v>
       </c>
@@ -2948,6 +3311,15 @@
       <c r="E36" t="s">
         <v>50</v>
       </c>
+      <c r="F36" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H36" s="2">
+        <v>14806</v>
+      </c>
       <c r="I36" t="s">
         <v>51</v>
       </c>
@@ -2968,6 +3340,15 @@
       <c r="E37" t="s">
         <v>52</v>
       </c>
+      <c r="F37" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H37" s="2">
+        <v>14606</v>
+      </c>
       <c r="I37" t="s">
         <v>53</v>
       </c>
@@ -2988,6 +3369,15 @@
       <c r="E38" t="s">
         <v>54</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H38" s="2">
+        <v>12180</v>
+      </c>
       <c r="I38" t="s">
         <v>55</v>
       </c>
@@ -3008,6 +3398,15 @@
       <c r="E39" t="s">
         <v>56</v>
       </c>
+      <c r="F39" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H39" s="2">
+        <v>14589</v>
+      </c>
       <c r="I39" t="s">
         <v>57</v>
       </c>
@@ -3028,6 +3427,15 @@
       <c r="E40" t="s">
         <v>58</v>
       </c>
+      <c r="F40" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H40" s="2">
+        <v>14505</v>
+      </c>
       <c r="I40" t="s">
         <v>59</v>
       </c>
@@ -3048,6 +3456,15 @@
       <c r="E41" t="s">
         <v>60</v>
       </c>
+      <c r="F41" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H41" s="2">
+        <v>10312</v>
+      </c>
       <c r="I41" t="s">
         <v>61</v>
       </c>
@@ -3068,6 +3485,15 @@
       <c r="E42" t="s">
         <v>62</v>
       </c>
+      <c r="F42" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H42" s="2">
+        <v>12309</v>
+      </c>
       <c r="I42" t="s">
         <v>63</v>
       </c>
@@ -3088,6 +3514,15 @@
       <c r="E43" t="s">
         <v>64</v>
       </c>
+      <c r="F43" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H43" s="2">
+        <v>12777</v>
+      </c>
       <c r="I43" t="s">
         <v>65</v>
       </c>
@@ -3108,6 +3543,15 @@
       <c r="E44" t="s">
         <v>66</v>
       </c>
+      <c r="F44" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H44" s="2">
+        <v>14505</v>
+      </c>
       <c r="I44" t="s">
         <v>67</v>
       </c>
@@ -3128,6 +3572,15 @@
       <c r="E45" t="s">
         <v>68</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H45" s="2">
+        <v>11710</v>
+      </c>
       <c r="I45" t="s">
         <v>69</v>
       </c>
@@ -3147,6 +3600,15 @@
       </c>
       <c r="E46" t="s">
         <v>191</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H46" s="2">
+        <v>14526</v>
       </c>
       <c r="I46" t="s">
         <v>192</v>

</xml_diff>

<commit_message>
added price per square foot
</commit_message>
<xml_diff>
--- a/property_listings.xlsx
+++ b/property_listings.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb0c59427c879960/Dokumenty/UiPath/Robot4_RealEstateScraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="575" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03A32695-B519-4340-B03F-AD440D60B49A}"/>
+  <xr:revisionPtr revIDLastSave="638" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F845188-CEC2-4C17-B29D-BDC487645A62}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{68A3964E-AA14-4F84-AC08-D41D65EA135C}"/>
   </bookViews>
   <sheets>
     <sheet name="SEATTLE" sheetId="4" r:id="rId1"/>
-    <sheet name="NEW YORK" sheetId="12" r:id="rId2"/>
+    <sheet name="NEW YORK" sheetId="16" r:id="rId2"/>
     <sheet name="Arkusz1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="208">
   <si>
     <t>Price</t>
   </si>
@@ -47,195 +47,99 @@
     <t>Listing URL</t>
   </si>
   <si>
-    <t>65 Green Street, Hudson, NY 12534</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/65-Green-St-Hudson-NY-12534/29998429_zpid/</t>
   </si>
   <si>
-    <t>11 Clearwater Road, Highland, NY 12528</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/11-Clearwater-Rd-Lloyd-NY-12528/32847251_zpid/</t>
   </si>
   <si>
-    <t>4 Wilderness Road, Nissequogue, NY 11780</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/4-Wilderness-Rd-Saint-James-NY-11780/32679146_zpid/</t>
   </si>
   <si>
-    <t>133 Clearvale Dr, Cheektowaga, NY 14225</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/133-Clearvale-Dr-Cheektowaga-NY-14225/30286848_zpid/</t>
   </si>
   <si>
-    <t>89 Harvest Rd, Fairport, NY 14450</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/89-Harvest-Rd-Fairport-NY-14450/31015880_zpid/</t>
   </si>
   <si>
-    <t>48 Chapin St, Canandaigua, NY 14424</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/48-Chapin-St-Canandaigua-NY-14424/31875795_zpid/</t>
   </si>
   <si>
-    <t>329 E 9th St, Oswego, NY 13126</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/329-E-9th-St-Oswego-NY-13126/53761158_zpid/</t>
   </si>
   <si>
-    <t>7 Margaret Drive, Ballston Spa, NY 12020</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/7-Margaret-Dr-Ballston-Spa-NY-12020/32443506_zpid/</t>
   </si>
   <si>
-    <t>206 Sweetman Road, Ballston Spa, NY 12020</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/206-Sweetman-Rd-Ballston-Spa-NY-12020/32412623_zpid/</t>
   </si>
   <si>
-    <t>219 Aris Ave, Cheektowaga, NY 14206</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/219-Aris-Ave-Cheektowaga-NY-14206/30298098_zpid/</t>
   </si>
   <si>
-    <t>67 Brewster St, Staten Island, NY 10304</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/67-Brewster-St-Staten-Island-NY-10304/32284423_zpid/</t>
   </si>
   <si>
-    <t>201 Dale St, Syracuse, NY 13208</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/201-Dale-St-Syracuse-NY-13208/31654747_zpid/</t>
   </si>
   <si>
-    <t>305 Valley Green Dr, Penfield, NY 14526</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/305-Valley-Green-Dr-Penfield-NY-14526/31004236_zpid/</t>
   </si>
   <si>
-    <t>1097 Marcia Dr, North Tonawanda, NY 14120</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/1097-Marcia-Dr-North-Tonawanda-NY-14120/31456719_zpid/</t>
   </si>
   <si>
-    <t>6 Sheila Drive, Syosset, NY 11791</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/6-Sheila-Dr-Syosset-NY-11791/31132060_zpid/</t>
   </si>
   <si>
-    <t>19 White Fawn Run, Rochester, NY 14624</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/19-White-Fawn-Run-Rochester-NY-14624/30907565_zpid/</t>
   </si>
   <si>
-    <t>141 Brannon Ln, Webster, NY 14580</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/141-Brannon-Ln-Webster-NY-14580/31047368_zpid/</t>
   </si>
   <si>
-    <t>8210 Perrugia Ln, Clay, NY 13041</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/8210-Perrugia-Ln-Clay-NY-13041/31711361_zpid/</t>
   </si>
   <si>
-    <t>5626 Newhouse Rd, East Amherst, NY 14051</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/5626-Newhouse-Rd-East-Amherst-NY-14051/30309364_zpid/</t>
   </si>
   <si>
-    <t>7364 E Seneca Tpke, Manlius, NY 13104</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/7364-E-Seneca-Tpke-Manlius-NY-13104/2088899524_zpid/</t>
   </si>
   <si>
-    <t>166 Cayuga St, Groton, NY 13073</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/166-Cayuga-St-Groton-NY-13073/32820526_zpid/</t>
   </si>
   <si>
-    <t>54 Taylor Dr, Tonawanda, NY 14150</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/54-Taylor-Dr-Tonawanda-NY-14150/30229358_zpid/</t>
   </si>
   <si>
-    <t>1366 County Road 30, Andover, NY 14806</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/1366-County-Road-30-Andover-NY-14806/29622595_zpid/</t>
   </si>
   <si>
-    <t>21 Marc Mar Cir, Rochester, NY 14606</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/21-Marc-Mar-Cir-Rochester-NY-14606/60033266_zpid/</t>
   </si>
   <si>
-    <t>1302 Sausse Avenue, Troy, NY 12180</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/1302-Sausse-Ave-Troy-NY-12180/32235275_zpid/</t>
   </si>
   <si>
-    <t>6778 Lake Ave, Williamson, NY 14589</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/6778-Lake-Ave-Williamson-NY-14589/32917619_zpid/</t>
   </si>
   <si>
-    <t>4057 Ridge Chapel Rd, Marion, NY 14505</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/4057-Ridge-Chapel-Rd-Marion-NY-14505/32910232_zpid/</t>
   </si>
   <si>
-    <t>308 Poillon Ave, Staten Island, NY 10312</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/308-Poillon-Ave-Staten-Island-NY-10312/2085654500_zpid/</t>
   </si>
   <si>
-    <t>74 Birchwood Lane, Schenectady, NY 12309</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/74-Birchwood-Ln-Schenectady-NY-12309/29681857_zpid/</t>
   </si>
   <si>
-    <t>1289 Plank Road, Forestburgh, NY 12777</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/1289-Plank-Rd-Forestburgh-NY-12777/32769930_zpid/</t>
   </si>
   <si>
-    <t>4575 Ridge Chapel Rd, Marion, NY 14505</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/4575-Ridge-Chapel-Rd-Marion-NY-14505/32910144_zpid/</t>
   </si>
   <si>
-    <t>407 Clinton St, Bellmore, NY 11710</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/407-Clinton-St-Bellmore-NY-11710/31391830_zpid/</t>
   </si>
   <si>
@@ -548,63 +452,12 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>3856 Stalker Rd, Macedon, NY 14502</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/3856-Stalker-Rd-Macedon-NY-14502/32914300_zpid/</t>
   </si>
   <si>
-    <t>30 Redbud Ct, East Amherst, NY 14051</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/30-Redbud-Ct-East-Amherst-NY-14051/30237744_zpid/</t>
   </si>
   <si>
-    <t>31 Meadow Dr, Big Flats, NY 14814</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/31-Meadow-Dr-Big-Flats-NY-14814/29962420_zpid/</t>
-  </si>
-  <si>
-    <t>36 Hathaway Rd, Rochester, NY 14617</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/36-Hathaway-Rd-Rochester-NY-14617/30970923_zpid/</t>
-  </si>
-  <si>
-    <t>1 Sunset Dr, Avon, NY 14414</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/1-Sunset-Dr-Avon-NY-14414/30806321_zpid/</t>
-  </si>
-  <si>
-    <t>66 Pickerel Road, Monroe, NY 10950</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/66-Pickerel-Rd-Monroe-NY-10950/31807123_zpid/</t>
-  </si>
-  <si>
-    <t>107 S Lincoln Ave, Liverpool, NY 13088</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/107-S-Lincoln-Ave-Liverpool-NY-13088/31769015_zpid/</t>
-  </si>
-  <si>
-    <t>4965 Driftwood Dr, Liverpool, NY 13088</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/4965-Driftwood-Dr-Liverpool-NY-13088/31770755_zpid/</t>
-  </si>
-  <si>
-    <t>214 Ardmore Street, Endicott, NY 13760</t>
-  </si>
-  <si>
-    <t>https://www.zillow.com/homedetails/214-Ardmore-St-Endicott-NY-13760/29764926_zpid/</t>
-  </si>
-  <si>
-    <t>114 Fiddlers Holw, Penfield, NY 14526</t>
-  </si>
-  <si>
     <t>https://www.zillow.com/homedetails/114-Fiddlers-Holw-Penfield-NY-14526/70904967_zpid/</t>
   </si>
   <si>
@@ -632,15 +485,6 @@
     <t>30 Redbud Ct</t>
   </si>
   <si>
-    <t>31 Meadow Dr</t>
-  </si>
-  <si>
-    <t>36 Hathaway Rd</t>
-  </si>
-  <si>
-    <t>1 Sunset Dr</t>
-  </si>
-  <si>
     <t>Hudson</t>
   </si>
   <si>
@@ -665,39 +509,12 @@
     <t>East Amherst</t>
   </si>
   <si>
-    <t>Big Flats</t>
-  </si>
-  <si>
     <t>Rochester</t>
   </si>
   <si>
-    <t>Avon</t>
-  </si>
-  <si>
-    <t>66 Pickerel Road</t>
-  </si>
-  <si>
-    <t>Monroe</t>
-  </si>
-  <si>
-    <t>107 S Lincoln Ave</t>
-  </si>
-  <si>
-    <t>Liverpool</t>
-  </si>
-  <si>
-    <t>4965 Driftwood Dr</t>
-  </si>
-  <si>
     <t>5626 Newhouse Rd</t>
   </si>
   <si>
-    <t>214 Ardmore Street</t>
-  </si>
-  <si>
-    <t>Endicott</t>
-  </si>
-  <si>
     <t>329 E 9th St</t>
   </si>
   <si>
@@ -831,6 +648,9 @@
   </si>
   <si>
     <t>114 Fiddlers Holw</t>
+  </si>
+  <si>
+    <t>Price per Sqft</t>
   </si>
 </sst>
 </file>
@@ -875,9 +695,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -905,6 +726,22 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person10.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person11.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person12.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person13.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1277,10 +1114,10 @@
         <v>702</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1297,10 +1134,10 @@
         <v>1081</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,10 +1154,10 @@
         <v>3674</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,10 +1174,10 @@
         <v>7362</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,10 +1194,10 @@
         <v>2060</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1377,10 +1214,10 @@
         <v>2460</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,10 +1234,10 @@
         <v>1150</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1417,10 +1254,10 @@
         <v>1097</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,10 +1274,10 @@
         <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1457,10 +1294,10 @@
         <v>1820</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1477,10 +1314,10 @@
         <v>1710</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1497,10 +1334,10 @@
         <v>1196</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1517,10 +1354,10 @@
         <v>1600</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,10 +1374,10 @@
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1557,10 +1394,10 @@
         <v>2000</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1577,10 +1414,10 @@
         <v>990</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1597,10 +1434,10 @@
         <v>2845</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1617,10 +1454,10 @@
         <v>1840</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,10 +1474,10 @@
         <v>3080</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1657,10 +1494,10 @@
         <v>2700</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1677,10 +1514,10 @@
         <v>2210</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1697,10 +1534,10 @@
         <v>2640</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1717,10 +1554,10 @@
         <v>640</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1737,10 +1574,10 @@
         <v>3703</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1757,10 +1594,10 @@
         <v>2830</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,10 +1614,10 @@
         <v>1550</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,10 +1634,10 @@
         <v>4400</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="F28" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,10 +1654,10 @@
         <v>852</v>
       </c>
       <c r="E29" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1837,10 +1674,10 @@
         <v>2660</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,10 +1694,10 @@
         <v>550</v>
       </c>
       <c r="E31" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="F31" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1877,10 +1714,10 @@
         <v>2800</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1897,10 +1734,10 @@
         <v>1400</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,10 +1754,10 @@
         <v>650</v>
       </c>
       <c r="E34" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1937,10 +1774,10 @@
         <v>2018</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,10 +1794,10 @@
         <v>812</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="F36" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,10 +1814,10 @@
         <v>1200</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="F37" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,10 +1834,10 @@
         <v>420</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="F38" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2017,10 +1854,10 @@
         <v>1690</v>
       </c>
       <c r="E39" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="F39" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2037,10 +1874,10 @@
         <v>1530</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="F40" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2057,10 +1894,10 @@
         <v>1290</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="F41" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2077,10 +1914,10 @@
         <v>3556</v>
       </c>
       <c r="E42" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="F42" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,10 +1934,10 @@
         <v>2900</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,10 +1954,10 @@
         <v>1890</v>
       </c>
       <c r="E44" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="F44" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2137,10 +1974,10 @@
         <v>3584</v>
       </c>
       <c r="E45" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="F45" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,10 +1994,10 @@
         <v>1850</v>
       </c>
       <c r="E46" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="F46" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2177,10 +2014,10 @@
         <v>4227</v>
       </c>
       <c r="E47" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="F47" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2197,10 +2034,10 @@
         <v>1405</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="F48" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2217,10 +2054,10 @@
         <v>3390</v>
       </c>
       <c r="E49" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="F49" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,10 +2074,10 @@
         <v>1974</v>
       </c>
       <c r="E50" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="F50" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2257,10 +2094,10 @@
         <v>2660</v>
       </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="F51" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2269,15 +2106,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED6A5AB-D69D-4B16-979E-F1DDC0300BBB}">
-  <dimension ref="A1:I46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562C1464-96DA-4827-B976-89CD4B428E67}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2293,17 +2131,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E1" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>172</v>
+        <v>139</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2322,20 +2160,20 @@
       <c r="D2">
         <v>1700</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2">
+        <v>302.941176470588</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="3">
+        <v>12534</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H2" s="2">
-        <v>12534</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2351,20 +2189,20 @@
       <c r="D3">
         <v>3257</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
+      <c r="E3" s="2">
+        <v>260.97635861221897</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H3" s="2">
+        <v>153</v>
+      </c>
+      <c r="H3" s="3">
         <v>12528</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2380,20 +2218,20 @@
       <c r="D4">
         <v>4800</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
+      <c r="E4" s="2">
+        <v>291.45833333333297</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>195</v>
+        <v>146</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="2">
+        <v>154</v>
+      </c>
+      <c r="H4" s="3">
         <v>11780</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2409,20 +2247,20 @@
       <c r="D5">
         <v>1260</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
+      <c r="E5" s="2">
+        <v>118.96825396825299</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>196</v>
+        <v>147</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H5" s="2">
+        <v>155</v>
+      </c>
+      <c r="H5" s="3">
         <v>14225</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2438,20 +2276,20 @@
       <c r="D6">
         <v>1008</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
+      <c r="E6" s="2">
+        <v>197.420634920634</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H6" s="2">
+        <v>156</v>
+      </c>
+      <c r="H6" s="3">
         <v>14450</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2467,20 +2305,20 @@
       <c r="D7">
         <v>1968</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
+      <c r="E7" s="2">
+        <v>96.493902439024396</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>198</v>
+        <v>149</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H7" s="2">
+        <v>157</v>
+      </c>
+      <c r="H7" s="3">
         <v>14424</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2496,20 +2334,20 @@
       <c r="D8">
         <v>1408</v>
       </c>
-      <c r="E8" t="s">
-        <v>173</v>
+      <c r="E8" s="2">
+        <v>127.769886363636</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>199</v>
+        <v>150</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H8" s="2">
+        <v>158</v>
+      </c>
+      <c r="H8" s="3">
         <v>14502</v>
       </c>
       <c r="I8" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2525,83 +2363,83 @@
       <c r="D9">
         <v>2520</v>
       </c>
-      <c r="E9" t="s">
-        <v>175</v>
+      <c r="E9" s="2">
+        <v>99.1666666666666</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" s="2">
+        <v>159</v>
+      </c>
+      <c r="H9" s="3">
         <v>14051</v>
       </c>
       <c r="I9" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>219900</v>
+        <v>80000</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>2390</v>
-      </c>
-      <c r="E10" t="s">
-        <v>177</v>
+        <v>1240</v>
+      </c>
+      <c r="E10" s="2">
+        <v>64.516129032257993</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="H10" s="2">
-        <v>14814</v>
+        <v>163</v>
+      </c>
+      <c r="H10" s="3">
+        <v>13126</v>
       </c>
       <c r="I10" t="s">
-        <v>178</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>199000</v>
+        <v>229900</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1355</v>
-      </c>
-      <c r="E11" t="s">
-        <v>179</v>
+        <v>936</v>
+      </c>
+      <c r="E11" s="2">
+        <v>245.619658119658</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H11" s="2">
-        <v>14617</v>
+        <v>165</v>
+      </c>
+      <c r="H11" s="3">
+        <v>12020</v>
       </c>
       <c r="I11" t="s">
-        <v>180</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>199900</v>
+        <v>289900</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2610,230 +2448,230 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <v>1350</v>
-      </c>
-      <c r="E12" t="s">
-        <v>181</v>
+        <v>1332</v>
+      </c>
+      <c r="E12" s="2">
+        <v>217.64264264264199</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H12" s="2">
-        <v>14414</v>
+        <v>165</v>
+      </c>
+      <c r="H12" s="3">
+        <v>12020</v>
       </c>
       <c r="I12" t="s">
-        <v>182</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>515000</v>
+        <v>179900</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1700</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
+        <v>990</v>
+      </c>
+      <c r="E13" s="2">
+        <v>181.717171717171</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H13" s="2">
-        <v>12534</v>
+        <v>155</v>
+      </c>
+      <c r="H13" s="3">
+        <v>14206</v>
       </c>
       <c r="I13" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>300000</v>
+        <v>748000</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>2148</v>
-      </c>
-      <c r="E14" t="s">
-        <v>183</v>
+        <v>2227</v>
+      </c>
+      <c r="E14" s="2">
+        <v>335.877862595419</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>215</v>
+        <v>168</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H14" s="2">
-        <v>10950</v>
+        <v>169</v>
+      </c>
+      <c r="H14" s="3">
+        <v>10304</v>
       </c>
       <c r="I14" t="s">
-        <v>184</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>186000</v>
+        <v>159900</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1080</v>
-      </c>
-      <c r="E15" t="s">
-        <v>185</v>
+        <v>1188</v>
+      </c>
+      <c r="E15" s="2">
+        <v>134.59595959595899</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>217</v>
+        <v>170</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H15" s="2">
-        <v>13088</v>
+        <v>171</v>
+      </c>
+      <c r="H15" s="3">
+        <v>13208</v>
       </c>
       <c r="I15" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>186000</v>
+        <v>279000</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>1080</v>
-      </c>
-      <c r="E16" t="s">
-        <v>185</v>
+        <v>1824</v>
+      </c>
+      <c r="E16" s="2">
+        <v>152.960526315789</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H16" s="2">
-        <v>13088</v>
+        <v>173</v>
+      </c>
+      <c r="H16" s="3">
+        <v>14526</v>
       </c>
       <c r="I16" t="s">
-        <v>186</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>189900</v>
+        <v>199900</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>936</v>
-      </c>
-      <c r="E17" t="s">
-        <v>187</v>
+        <v>1222</v>
+      </c>
+      <c r="E17" s="2">
+        <v>163.58428805237301</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H17" s="2">
-        <v>13088</v>
+        <v>175</v>
+      </c>
+      <c r="H17" s="3">
+        <v>14120</v>
       </c>
       <c r="I17" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>199900</v>
+        <v>1100000</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>960</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
+        <v>2659</v>
+      </c>
+      <c r="E18" s="2">
+        <v>413.68935690108998</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H18" s="2">
-        <v>14051</v>
+        <v>177</v>
+      </c>
+      <c r="H18" s="3">
+        <v>11791</v>
       </c>
       <c r="I18" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>169000</v>
+        <v>250000</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19">
-        <v>1152</v>
-      </c>
-      <c r="E19" t="s">
-        <v>189</v>
+        <v>1789</v>
+      </c>
+      <c r="E19" s="2">
+        <v>139.74287311347101</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H19" s="2">
-        <v>13760</v>
+        <v>160</v>
+      </c>
+      <c r="H19" s="3">
+        <v>14624</v>
       </c>
       <c r="I19" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>80000</v>
+        <v>289900</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2842,106 +2680,106 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>1240</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
+        <v>1347</v>
+      </c>
+      <c r="E20" s="2">
+        <v>215.21900519673301</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H20" s="2">
-        <v>13126</v>
+        <v>180</v>
+      </c>
+      <c r="H20" s="3">
+        <v>14580</v>
       </c>
       <c r="I20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>229900</v>
+        <v>285000</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>936</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
+        <v>1400</v>
+      </c>
+      <c r="E21" s="2">
+        <v>203.57142857142799</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H21" s="2">
-        <v>12020</v>
+        <v>182</v>
+      </c>
+      <c r="H21" s="3">
+        <v>13041</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>289900</v>
+        <v>199900</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1332</v>
-      </c>
-      <c r="E22" t="s">
-        <v>22</v>
+        <v>960</v>
+      </c>
+      <c r="E22" s="2">
+        <v>208.229166666666</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H22" s="2">
-        <v>12020</v>
+        <v>159</v>
+      </c>
+      <c r="H22" s="3">
+        <v>14051</v>
       </c>
       <c r="I22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>179900</v>
+        <v>369900</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>990</v>
-      </c>
-      <c r="E23" t="s">
-        <v>24</v>
+        <v>2450</v>
+      </c>
+      <c r="E23" s="2">
+        <v>150.97959183673399</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H23" s="2">
-        <v>14206</v>
+        <v>184</v>
+      </c>
+      <c r="H23" s="3">
+        <v>13104</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -2949,326 +2787,326 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>748000</v>
+        <v>248000</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>2227</v>
-      </c>
-      <c r="E24" t="s">
+        <v>1666</v>
+      </c>
+      <c r="E24" s="2">
+        <v>148.859543817527</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H24" s="3">
+        <v>13073</v>
+      </c>
+      <c r="I24" t="s">
         <v>26</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="H24" s="2">
-        <v>10304</v>
-      </c>
-      <c r="I24" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>159900</v>
+        <v>249900</v>
       </c>
       <c r="B25">
         <v>3</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>1188</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
+        <v>1324</v>
+      </c>
+      <c r="E25" s="2">
+        <v>188.74622356495399</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H25" s="2">
-        <v>13208</v>
+        <v>188</v>
+      </c>
+      <c r="H25" s="3">
+        <v>14150</v>
       </c>
       <c r="I25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>279000</v>
+        <v>164900</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>1824</v>
-      </c>
-      <c r="E26" t="s">
-        <v>30</v>
+        <v>1656</v>
+      </c>
+      <c r="E26" s="2">
+        <v>99.577294685990296</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H26" s="2">
-        <v>14526</v>
+        <v>190</v>
+      </c>
+      <c r="H26" s="3">
+        <v>14806</v>
       </c>
       <c r="I26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>199900</v>
+        <v>389900</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>1222</v>
-      </c>
-      <c r="E27" t="s">
-        <v>32</v>
+        <v>2738</v>
+      </c>
+      <c r="E27" s="2">
+        <v>142.40321402483499</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H27" s="2">
-        <v>14120</v>
+        <v>160</v>
+      </c>
+      <c r="H27" s="3">
+        <v>14606</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1100000</v>
+        <v>264900</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>2659</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
+        <v>1700</v>
+      </c>
+      <c r="E28" s="2">
+        <v>155.82352941176401</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H28" s="2">
-        <v>11791</v>
+        <v>193</v>
+      </c>
+      <c r="H28" s="3">
+        <v>12180</v>
       </c>
       <c r="I28" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>250000</v>
+        <v>149900</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>1789</v>
-      </c>
-      <c r="E29" t="s">
-        <v>36</v>
+        <v>1547</v>
+      </c>
+      <c r="E29" s="2">
+        <v>96.897220426632103</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H29" s="2">
-        <v>14624</v>
+        <v>195</v>
+      </c>
+      <c r="H29" s="3">
+        <v>14589</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>289900</v>
+        <v>99900</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30">
-        <v>1347</v>
-      </c>
-      <c r="E30" t="s">
-        <v>38</v>
+        <v>1966</v>
+      </c>
+      <c r="E30" s="2">
+        <v>50.813835198372303</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>240</v>
+        <v>196</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H30" s="2">
-        <v>14580</v>
+        <v>197</v>
+      </c>
+      <c r="H30" s="3">
+        <v>14505</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>285000</v>
+        <v>1388000</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>1400</v>
-      </c>
-      <c r="E31" t="s">
-        <v>40</v>
+        <v>2700</v>
+      </c>
+      <c r="E31" s="2">
+        <v>514.07407407407402</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>242</v>
+        <v>198</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="H31" s="2">
-        <v>13041</v>
+        <v>169</v>
+      </c>
+      <c r="H31" s="3">
+        <v>10312</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>199900</v>
+        <v>225000</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>960</v>
-      </c>
-      <c r="E32" t="s">
-        <v>42</v>
+        <v>1408</v>
+      </c>
+      <c r="E32" s="2">
+        <v>159.801136363636</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H32" s="2">
-        <v>14051</v>
+        <v>200</v>
+      </c>
+      <c r="H32" s="3">
+        <v>12309</v>
       </c>
       <c r="I32" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>369900</v>
+        <v>699000</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>2450</v>
-      </c>
-      <c r="E33" t="s">
-        <v>44</v>
+        <v>2040</v>
+      </c>
+      <c r="E33" s="2">
+        <v>342.64705882352899</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="H33" s="2">
-        <v>13104</v>
+        <v>202</v>
+      </c>
+      <c r="H33" s="3">
+        <v>12777</v>
       </c>
       <c r="I33" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>248000</v>
+        <v>209900</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>1666</v>
-      </c>
-      <c r="E34" t="s">
-        <v>46</v>
+        <v>1800</v>
+      </c>
+      <c r="E34" s="2">
+        <v>116.611111111111</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>246</v>
+        <v>203</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H34" s="2">
-        <v>13073</v>
+        <v>197</v>
+      </c>
+      <c r="H34" s="3">
+        <v>14505</v>
       </c>
       <c r="I34" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>249900</v>
+        <v>255000</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -3277,341 +3115,51 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <v>1324</v>
-      </c>
-      <c r="E35" t="s">
-        <v>48</v>
+        <v>1428</v>
+      </c>
+      <c r="E35" s="2">
+        <v>178.57142857142799</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>248</v>
+        <v>204</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="H35" s="2">
-        <v>14150</v>
+        <v>205</v>
+      </c>
+      <c r="H35" s="3">
+        <v>11710</v>
       </c>
       <c r="I35" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>164900</v>
+        <v>579900</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>1656</v>
-      </c>
-      <c r="E36" t="s">
-        <v>50</v>
+        <v>3191</v>
+      </c>
+      <c r="E36" s="2">
+        <v>181.72986524600401</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="H36" s="2">
-        <v>14806</v>
+        <v>173</v>
+      </c>
+      <c r="H36" s="3">
+        <v>14526</v>
       </c>
       <c r="I36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>389900</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>2738</v>
-      </c>
-      <c r="E37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H37" s="2">
-        <v>14606</v>
-      </c>
-      <c r="I37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>264900</v>
-      </c>
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <v>1700</v>
-      </c>
-      <c r="E38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="H38" s="2">
-        <v>12180</v>
-      </c>
-      <c r="I38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>149900</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>1547</v>
-      </c>
-      <c r="E39" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="H39" s="2">
-        <v>14589</v>
-      </c>
-      <c r="I39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>99900</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
-        <v>1966</v>
-      </c>
-      <c r="E40" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="H40" s="2">
-        <v>14505</v>
-      </c>
-      <c r="I40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1388000</v>
-      </c>
-      <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41">
-        <v>4</v>
-      </c>
-      <c r="D41">
-        <v>2700</v>
-      </c>
-      <c r="E41" t="s">
-        <v>60</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="H41" s="2">
-        <v>10312</v>
-      </c>
-      <c r="I41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>225000</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>1408</v>
-      </c>
-      <c r="E42" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H42" s="2">
-        <v>12309</v>
-      </c>
-      <c r="I42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>699000</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>2040</v>
-      </c>
-      <c r="E43" t="s">
-        <v>64</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H43" s="2">
-        <v>12777</v>
-      </c>
-      <c r="I43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>209900</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44">
-        <v>1800</v>
-      </c>
-      <c r="E44" t="s">
-        <v>66</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="H44" s="2">
-        <v>14505</v>
-      </c>
-      <c r="I44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>255000</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>1428</v>
-      </c>
-      <c r="E45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="H45" s="2">
-        <v>11710</v>
-      </c>
-      <c r="I45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>579900</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-      <c r="D46">
-        <v>3191</v>
-      </c>
-      <c r="E46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H46" s="2">
-        <v>14526</v>
-      </c>
-      <c r="I46" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sorting by beds and baths
</commit_message>
<xml_diff>
--- a/property_listings.xlsx
+++ b/property_listings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb0c59427c879960/Dokumenty/UiPath/Robot4_RealEstateScraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="638" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F845188-CEC2-4C17-B29D-BDC487645A62}"/>
+  <xr:revisionPtr revIDLastSave="641" documentId="8_{75E2279D-B3D6-478C-962E-1CE9EC85018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{752EBE94-D946-4F37-896E-681ACADC2ACB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{68A3964E-AA14-4F84-AC08-D41D65EA135C}"/>
   </bookViews>
@@ -699,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -742,6 +742,10 @@
 </file>
 
 <file path=xl/persons/person13.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person14.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2149,7 +2153,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>515000</v>
+        <v>99900</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -2158,80 +2162,80 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>1700</v>
+        <v>1966</v>
       </c>
       <c r="E2" s="2">
-        <v>302.941176470588</v>
+        <v>50.813835198372303</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="H2" s="3">
-        <v>12534</v>
+        <v>14505</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>850000</v>
+        <v>80000</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>3257</v>
+        <v>1240</v>
       </c>
       <c r="E3" s="2">
-        <v>260.97635861221897</v>
+        <v>64.516129032257993</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="H3" s="3">
-        <v>12528</v>
+        <v>13126</v>
       </c>
       <c r="I3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1399000</v>
+        <v>189900</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>4800</v>
+        <v>1968</v>
       </c>
       <c r="E4" s="2">
-        <v>291.45833333333297</v>
+        <v>96.493902439024396</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H4" s="3">
-        <v>11780</v>
+        <v>14424</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2239,62 +2243,62 @@
         <v>149900</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1260</v>
+        <v>1547</v>
       </c>
       <c r="E5" s="2">
-        <v>118.96825396825299</v>
+        <v>96.897220426632103</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="H5" s="3">
-        <v>14225</v>
+        <v>14589</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>199000</v>
+        <v>249900</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>1008</v>
+        <v>2520</v>
       </c>
       <c r="E6" s="2">
-        <v>197.420634920634</v>
+        <v>99.1666666666666</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H6" s="3">
-        <v>14450</v>
+        <v>14051</v>
       </c>
       <c r="I6" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>189900</v>
+        <v>164900</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2303,114 +2307,114 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>1968</v>
+        <v>1656</v>
       </c>
       <c r="E7" s="2">
-        <v>96.493902439024396</v>
+        <v>99.577294685990296</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="H7" s="3">
-        <v>14424</v>
+        <v>14806</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>179900</v>
+        <v>209900</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>1408</v>
+        <v>1800</v>
       </c>
       <c r="E8" s="2">
-        <v>127.769886363636</v>
+        <v>116.611111111111</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>150</v>
+        <v>203</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="H8" s="3">
-        <v>14502</v>
+        <v>14505</v>
       </c>
       <c r="I8" t="s">
-        <v>141</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>249900</v>
+        <v>149900</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2520</v>
+        <v>1260</v>
       </c>
       <c r="E9" s="2">
-        <v>99.1666666666666</v>
+        <v>118.96825396825299</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H9" s="3">
-        <v>14051</v>
+        <v>14225</v>
       </c>
       <c r="I9" t="s">
-        <v>142</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>80000</v>
+        <v>179900</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1240</v>
+        <v>1408</v>
       </c>
       <c r="E10" s="2">
-        <v>64.516129032257993</v>
+        <v>127.769886363636</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H10" s="3">
-        <v>13126</v>
+        <v>14502</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>229900</v>
+        <v>159900</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -2419,138 +2423,138 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>936</v>
+        <v>1188</v>
       </c>
       <c r="E11" s="2">
-        <v>245.619658119658</v>
+        <v>134.59595959595899</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="H11" s="3">
-        <v>12020</v>
+        <v>13208</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>289900</v>
+        <v>250000</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>1332</v>
+        <v>1789</v>
       </c>
       <c r="E12" s="2">
-        <v>217.64264264264199</v>
+        <v>139.74287311347101</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H12" s="3">
-        <v>12020</v>
+        <v>14624</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>179900</v>
+        <v>389900</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>990</v>
+        <v>2738</v>
       </c>
       <c r="E13" s="2">
-        <v>181.717171717171</v>
+        <v>142.40321402483499</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="H13" s="3">
-        <v>14206</v>
+        <v>14606</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>748000</v>
+        <v>248000</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>2227</v>
+        <v>1666</v>
       </c>
       <c r="E14" s="2">
-        <v>335.877862595419</v>
+        <v>148.859543817527</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="H14" s="3">
-        <v>10304</v>
+        <v>13073</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>159900</v>
+        <v>369900</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>1188</v>
+        <v>2450</v>
       </c>
       <c r="E15" s="2">
-        <v>134.59595959595899</v>
+        <v>150.97959183673399</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="H15" s="3">
-        <v>13208</v>
+        <v>13104</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2584,94 +2588,94 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>199900</v>
+        <v>264900</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17">
-        <v>1222</v>
+        <v>1700</v>
       </c>
       <c r="E17" s="2">
-        <v>163.58428805237301</v>
+        <v>155.82352941176401</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="H17" s="3">
-        <v>14120</v>
+        <v>12180</v>
       </c>
       <c r="I17" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1100000</v>
+        <v>225000</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>2659</v>
+        <v>1408</v>
       </c>
       <c r="E18" s="2">
-        <v>413.68935690108998</v>
+        <v>159.801136363636</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="H18" s="3">
-        <v>11791</v>
+        <v>12309</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>250000</v>
+        <v>199900</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19">
-        <v>1789</v>
+        <v>1222</v>
       </c>
       <c r="E19" s="2">
-        <v>139.74287311347101</v>
+        <v>163.58428805237301</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="H19" s="3">
-        <v>14624</v>
+        <v>14120</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>289900</v>
+        <v>255000</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -2680,114 +2684,114 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>1347</v>
+        <v>1428</v>
       </c>
       <c r="E20" s="2">
-        <v>215.21900519673301</v>
+        <v>178.57142857142799</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="H20" s="3">
-        <v>14580</v>
+        <v>11710</v>
       </c>
       <c r="I20" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>285000</v>
+        <v>179900</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>1400</v>
+        <v>990</v>
       </c>
       <c r="E21" s="2">
-        <v>203.57142857142799</v>
+        <v>181.717171717171</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="H21" s="3">
-        <v>13041</v>
+        <v>14206</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>199900</v>
+        <v>579900</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>960</v>
+        <v>3191</v>
       </c>
       <c r="E22" s="2">
-        <v>208.229166666666</v>
+        <v>181.72986524600401</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>161</v>
+        <v>206</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="H22" s="3">
-        <v>14051</v>
+        <v>14526</v>
       </c>
       <c r="I22" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>369900</v>
+        <v>249900</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>2450</v>
+        <v>1324</v>
       </c>
       <c r="E23" s="2">
-        <v>150.97959183673399</v>
+        <v>188.74622356495399</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H23" s="3">
-        <v>13104</v>
+        <v>14150</v>
       </c>
       <c r="I23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>248000</v>
+        <v>199000</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2796,143 +2800,143 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>1666</v>
+        <v>1008</v>
       </c>
       <c r="E24" s="2">
-        <v>148.859543817527</v>
+        <v>197.420634920634</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="H24" s="3">
-        <v>13073</v>
+        <v>14450</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>249900</v>
+        <v>285000</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25">
-        <v>1324</v>
+        <v>1400</v>
       </c>
       <c r="E25" s="2">
-        <v>188.74622356495399</v>
+        <v>203.57142857142799</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H25" s="3">
-        <v>14150</v>
+        <v>13041</v>
       </c>
       <c r="I25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>164900</v>
+        <v>199900</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1656</v>
+        <v>960</v>
       </c>
       <c r="E26" s="2">
-        <v>99.577294685990296</v>
+        <v>208.229166666666</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="H26" s="3">
-        <v>14806</v>
+        <v>14051</v>
       </c>
       <c r="I26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>389900</v>
+        <v>289900</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>2738</v>
+        <v>1347</v>
       </c>
       <c r="E27" s="2">
-        <v>142.40321402483499</v>
+        <v>215.21900519673301</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="H27" s="3">
-        <v>14606</v>
+        <v>14580</v>
       </c>
       <c r="I27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>264900</v>
+        <v>289900</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28">
-        <v>1700</v>
+        <v>1332</v>
       </c>
       <c r="E28" s="2">
-        <v>155.82352941176401</v>
+        <v>217.64264264264199</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="H28" s="3">
-        <v>12180</v>
+        <v>12020</v>
       </c>
       <c r="I28" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>149900</v>
+        <v>229900</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2941,85 +2945,85 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1547</v>
+        <v>936</v>
       </c>
       <c r="E29" s="2">
-        <v>96.897220426632103</v>
+        <v>245.619658119658</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="H29" s="3">
-        <v>14589</v>
+        <v>12020</v>
       </c>
       <c r="I29" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>99900</v>
+        <v>850000</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>1966</v>
+        <v>3257</v>
       </c>
       <c r="E30" s="2">
-        <v>50.813835198372303</v>
+        <v>260.97635861221897</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="H30" s="3">
-        <v>14505</v>
+        <v>12528</v>
       </c>
       <c r="I30" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1388000</v>
+        <v>1399000</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31">
-        <v>2700</v>
+        <v>4800</v>
       </c>
       <c r="E31" s="2">
-        <v>514.07407407407402</v>
+        <v>291.45833333333297</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H31" s="3">
-        <v>10312</v>
+        <v>11780</v>
       </c>
       <c r="I31" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>225000</v>
+        <v>515000</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -3028,141 +3032,144 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <v>1408</v>
+        <v>1700</v>
       </c>
       <c r="E32" s="2">
-        <v>159.801136363636</v>
+        <v>302.941176470588</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>199</v>
+        <v>144</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="H32" s="3">
-        <v>12309</v>
+        <v>12534</v>
       </c>
       <c r="I32" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>699000</v>
+        <v>748000</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33">
-        <v>2040</v>
+        <v>2227</v>
       </c>
       <c r="E33" s="2">
-        <v>342.64705882352899</v>
+        <v>335.877862595419</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="H33" s="3">
-        <v>12777</v>
+        <v>10304</v>
       </c>
       <c r="I33" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>209900</v>
+        <v>699000</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>1800</v>
+        <v>2040</v>
       </c>
       <c r="E34" s="2">
-        <v>116.611111111111</v>
+        <v>342.64705882352899</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="H34" s="3">
-        <v>14505</v>
+        <v>12777</v>
       </c>
       <c r="I34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>255000</v>
+        <v>1100000</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35">
-        <v>1428</v>
+        <v>2659</v>
       </c>
       <c r="E35" s="2">
-        <v>178.57142857142799</v>
+        <v>413.68935690108998</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="H35" s="3">
-        <v>11710</v>
+        <v>11791</v>
       </c>
       <c r="I35" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>579900</v>
+        <v>1388000</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>3191</v>
+        <v>2700</v>
       </c>
       <c r="E36" s="2">
-        <v>181.72986524600401</v>
+        <v>514.07407407407402</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H36" s="3">
-        <v>14526</v>
+        <v>10312</v>
       </c>
       <c r="I36" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>